<commit_message>
landing page and loading screen students
</commit_message>
<xml_diff>
--- a/translations/config.xlsx
+++ b/translations/config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\SP_Project\translations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33703F41-E751-4A31-8F5B-67F67111E721}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEB55DC-300D-451A-8576-4AD35D94BBB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{05EE6742-DC1F-4D30-8912-AFBDF4D1E2A6}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Feuil2 (2)" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$C$338</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$C$339</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,6 +28,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="744">
   <si>
     <t>clé</t>
   </si>
@@ -2274,6 +2280,15 @@
   </si>
   <si>
     <t>scolarité</t>
+  </si>
+  <si>
+    <t>loading screen</t>
+  </si>
+  <si>
+    <t>loading please wait…</t>
+  </si>
+  <si>
+    <t>Patientez pendant le chargement…</t>
   </si>
 </sst>
 </file>
@@ -2285,7 +2300,7 @@
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2596,9 +2611,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA8BC614-FBAA-4786-803C-84330B31A162}" name="Tableau1" displayName="Tableau1" ref="A1:C338" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C338" xr:uid="{CE0DE1EE-6F35-4194-BA96-445580CA0C4B}"/>
-  <sortState ref="A35:C336">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA8BC614-FBAA-4786-803C-84330B31A162}" name="Tableau1" displayName="Tableau1" ref="A1:C339" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C339" xr:uid="{CE0DE1EE-6F35-4194-BA96-445580CA0C4B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:C336">
     <sortCondition ref="A1:A336"/>
   </sortState>
   <tableColumns count="3">
@@ -2907,14 +2922,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0DE1EE-6F35-4194-BA96-445580CA0C4B}">
-  <dimension ref="A1:C338"/>
+  <dimension ref="A1:C339"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C143" sqref="C143"/>
+      <pane ySplit="1" topLeftCell="A319" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B334" sqref="B334"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="28.5546875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="28.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="28.5546875" style="2"/>
     <col min="2" max="2" width="67.33203125" style="3" customWidth="1"/>
@@ -2922,7 +2937,7 @@
     <col min="4" max="16384" width="28.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="21.6" customHeight="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2933,7 +2948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>73</v>
       </c>
@@ -2944,7 +2959,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>172</v>
       </c>
@@ -2955,7 +2970,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>225</v>
       </c>
@@ -2966,7 +2981,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>530</v>
       </c>
@@ -2977,7 +2992,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>484</v>
       </c>
@@ -2988,7 +3003,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>522</v>
       </c>
@@ -2999,7 +3014,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>521</v>
       </c>
@@ -3010,7 +3025,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>523</v>
       </c>
@@ -3021,7 +3036,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>274</v>
       </c>
@@ -3032,7 +3047,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>246</v>
       </c>
@@ -3043,7 +3058,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>284</v>
       </c>
@@ -3054,7 +3069,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>207</v>
       </c>
@@ -3065,7 +3080,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>207</v>
       </c>
@@ -3076,7 +3091,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>197</v>
       </c>
@@ -3087,7 +3102,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>197</v>
       </c>
@@ -3098,7 +3113,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>209</v>
       </c>
@@ -3109,7 +3124,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>311</v>
       </c>
@@ -3120,7 +3135,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>358</v>
       </c>
@@ -3131,7 +3146,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>416</v>
       </c>
@@ -3142,7 +3157,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>380</v>
       </c>
@@ -3153,7 +3168,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>241</v>
       </c>
@@ -3164,7 +3179,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>550</v>
       </c>
@@ -3175,7 +3190,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -3186,7 +3201,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>466</v>
       </c>
@@ -3197,7 +3212,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>324</v>
       </c>
@@ -3208,7 +3223,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>429</v>
       </c>
@@ -3219,7 +3234,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>477</v>
       </c>
@@ -3230,7 +3245,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>384</v>
       </c>
@@ -3241,7 +3256,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>168</v>
       </c>
@@ -3252,7 +3267,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>112</v>
       </c>
@@ -3263,7 +3278,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
@@ -3274,7 +3289,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>402</v>
       </c>
@@ -3285,7 +3300,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>414</v>
       </c>
@@ -3296,7 +3311,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>303</v>
       </c>
@@ -3307,7 +3322,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>435</v>
       </c>
@@ -3318,7 +3333,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>363</v>
       </c>
@@ -3329,7 +3344,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>543</v>
       </c>
@@ -3340,7 +3355,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>491</v>
       </c>
@@ -3351,7 +3366,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>293</v>
       </c>
@@ -3362,7 +3377,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>134</v>
       </c>
@@ -3373,7 +3388,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>85</v>
       </c>
@@ -3384,7 +3399,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>271</v>
       </c>
@@ -3395,7 +3410,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>87</v>
       </c>
@@ -3406,7 +3421,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>70</v>
       </c>
@@ -3417,7 +3432,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>52</v>
       </c>
@@ -3428,7 +3443,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>473</v>
       </c>
@@ -3439,7 +3454,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>185</v>
       </c>
@@ -3450,7 +3465,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>309</v>
       </c>
@@ -3461,7 +3476,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>159</v>
       </c>
@@ -3472,7 +3487,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>183</v>
       </c>
@@ -3483,7 +3498,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>433</v>
       </c>
@@ -3494,7 +3509,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>166</v>
       </c>
@@ -3505,7 +3520,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>80</v>
       </c>
@@ -3516,7 +3531,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>318</v>
       </c>
@@ -3527,7 +3542,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>136</v>
       </c>
@@ -3538,7 +3553,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>336</v>
       </c>
@@ -3549,7 +3564,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>343</v>
       </c>
@@ -3560,7 +3575,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>344</v>
       </c>
@@ -3571,7 +3586,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>345</v>
       </c>
@@ -3582,7 +3597,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>346</v>
       </c>
@@ -3593,7 +3608,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>347</v>
       </c>
@@ -3604,7 +3619,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>544</v>
       </c>
@@ -3615,7 +3630,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>205</v>
       </c>
@@ -3626,7 +3641,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>315</v>
       </c>
@@ -3637,7 +3652,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>554</v>
       </c>
@@ -3648,7 +3663,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>361</v>
       </c>
@@ -3659,7 +3674,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>546</v>
       </c>
@@ -3670,7 +3685,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>82</v>
       </c>
@@ -3681,7 +3696,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>82</v>
       </c>
@@ -3692,7 +3707,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>373</v>
       </c>
@@ -3703,7 +3718,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>110</v>
       </c>
@@ -3714,7 +3729,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>6</v>
       </c>
@@ -3725,7 +3740,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>243</v>
       </c>
@@ -3736,7 +3751,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>94</v>
       </c>
@@ -3747,7 +3762,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>542</v>
       </c>
@@ -3758,7 +3773,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>302</v>
       </c>
@@ -3769,7 +3784,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>91</v>
       </c>
@@ -3780,7 +3795,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>573</v>
       </c>
@@ -3791,7 +3806,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>575</v>
       </c>
@@ -3802,7 +3817,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>174</v>
       </c>
@@ -3813,7 +3828,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>313</v>
       </c>
@@ -3824,7 +3839,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>3</v>
       </c>
@@ -3835,7 +3850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>495</v>
       </c>
@@ -3846,7 +3861,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>490</v>
       </c>
@@ -3857,7 +3872,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>213</v>
       </c>
@@ -3868,7 +3883,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>214</v>
       </c>
@@ -3879,7 +3894,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>532</v>
       </c>
@@ -3890,7 +3905,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>48</v>
       </c>
@@ -3901,7 +3916,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>58</v>
       </c>
@@ -3912,7 +3927,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>103</v>
       </c>
@@ -3923,7 +3938,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>282</v>
       </c>
@@ -3934,7 +3949,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>64</v>
       </c>
@@ -3945,7 +3960,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>68</v>
       </c>
@@ -3956,7 +3971,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>69</v>
       </c>
@@ -3967,7 +3982,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>99</v>
       </c>
@@ -3978,7 +3993,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>565</v>
       </c>
@@ -3989,7 +4004,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>162</v>
       </c>
@@ -4000,7 +4015,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>31</v>
       </c>
@@ -4011,7 +4026,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>534</v>
       </c>
@@ -4022,7 +4037,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>424</v>
       </c>
@@ -4033,7 +4048,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>312</v>
       </c>
@@ -4044,7 +4059,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>382</v>
       </c>
@@ -4055,7 +4070,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>378</v>
       </c>
@@ -4066,7 +4081,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>386</v>
       </c>
@@ -4077,7 +4092,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>152</v>
       </c>
@@ -4088,7 +4103,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>42</v>
       </c>
@@ -4099,7 +4114,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>325</v>
       </c>
@@ -4110,7 +4125,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>431</v>
       </c>
@@ -4121,7 +4136,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>55</v>
       </c>
@@ -4132,7 +4147,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>179</v>
       </c>
@@ -4143,7 +4158,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>104</v>
       </c>
@@ -4154,7 +4169,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>371</v>
       </c>
@@ -4165,7 +4180,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>412</v>
       </c>
@@ -4176,7 +4191,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>423</v>
       </c>
@@ -4187,7 +4202,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>181</v>
       </c>
@@ -4198,7 +4213,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>463</v>
       </c>
@@ -4209,7 +4224,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>299</v>
       </c>
@@ -4220,7 +4235,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>569</v>
       </c>
@@ -4231,7 +4246,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>228</v>
       </c>
@@ -4242,7 +4257,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>578</v>
       </c>
@@ -4253,7 +4268,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>295</v>
       </c>
@@ -4264,7 +4279,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>244</v>
       </c>
@@ -4275,7 +4290,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>449</v>
       </c>
@@ -4286,7 +4301,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>133</v>
       </c>
@@ -4297,7 +4312,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>305</v>
       </c>
@@ -4308,7 +4323,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>176</v>
       </c>
@@ -4319,7 +4334,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>156</v>
       </c>
@@ -4330,7 +4345,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>571</v>
       </c>
@@ -4341,7 +4356,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>148</v>
       </c>
@@ -4352,7 +4367,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>452</v>
       </c>
@@ -4363,7 +4378,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>307</v>
       </c>
@@ -4374,7 +4389,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>280</v>
       </c>
@@ -4385,7 +4400,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>97</v>
       </c>
@@ -4396,7 +4411,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>164</v>
       </c>
@@ -4407,7 +4422,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>426</v>
       </c>
@@ -4418,7 +4433,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>128</v>
       </c>
@@ -4429,7 +4444,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>120</v>
       </c>
@@ -4440,7 +4455,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>122</v>
       </c>
@@ -4451,7 +4466,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>126</v>
       </c>
@@ -4462,7 +4477,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="19.8" customHeight="1">
+    <row r="141" spans="1:3" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>131</v>
       </c>
@@ -4473,7 +4488,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>125</v>
       </c>
@@ -4484,7 +4499,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="143" spans="1:3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>121</v>
       </c>
@@ -4495,7 +4510,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>123</v>
       </c>
@@ -4506,7 +4521,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="145" spans="1:3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>124</v>
       </c>
@@ -4517,7 +4532,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>127</v>
       </c>
@@ -4528,7 +4543,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>450</v>
       </c>
@@ -4539,7 +4554,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="148" spans="1:3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>49</v>
       </c>
@@ -4550,7 +4565,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="149" spans="1:3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>38</v>
       </c>
@@ -4561,7 +4576,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="150" spans="1:3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>527</v>
       </c>
@@ -4572,7 +4587,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>461</v>
       </c>
@@ -4583,7 +4598,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="152" spans="1:3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>526</v>
       </c>
@@ -4594,7 +4609,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="153" spans="1:3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>236</v>
       </c>
@@ -4605,7 +4620,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>454</v>
       </c>
@@ -4616,7 +4631,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="155" spans="1:3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>211</v>
       </c>
@@ -4627,7 +4642,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="156" spans="1:3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>486</v>
       </c>
@@ -4638,7 +4653,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="157" spans="1:3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>261</v>
       </c>
@@ -4649,7 +4664,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>258</v>
       </c>
@@ -4660,7 +4675,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>388</v>
       </c>
@@ -4671,7 +4686,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="160" spans="1:3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>177</v>
       </c>
@@ -4682,7 +4697,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>145</v>
       </c>
@@ -4693,7 +4708,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="162" spans="1:3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>72</v>
       </c>
@@ -4704,7 +4719,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>188</v>
       </c>
@@ -4715,7 +4730,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="164" spans="1:3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>488</v>
       </c>
@@ -4726,7 +4741,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="165" spans="1:3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>367</v>
       </c>
@@ -4737,7 +4752,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="166" spans="1:3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>421</v>
       </c>
@@ -4748,7 +4763,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="167" spans="1:3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>235</v>
       </c>
@@ -4759,7 +4774,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="168" spans="1:3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>235</v>
       </c>
@@ -4770,7 +4785,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="169" spans="1:3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>561</v>
       </c>
@@ -4781,7 +4796,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="170" spans="1:3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>559</v>
       </c>
@@ -4792,7 +4807,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="171" spans="1:3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>551</v>
       </c>
@@ -4803,7 +4818,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>564</v>
       </c>
@@ -4814,7 +4829,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>525</v>
       </c>
@@ -4825,7 +4840,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="174" spans="1:3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>499</v>
       </c>
@@ -4836,7 +4851,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="175" spans="1:3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>287</v>
       </c>
@@ -4847,7 +4862,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>447</v>
       </c>
@@ -4858,7 +4873,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>150</v>
       </c>
@@ -4869,7 +4884,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>12</v>
       </c>
@@ -4880,7 +4895,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>62</v>
       </c>
@@ -4891,7 +4906,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>276</v>
       </c>
@@ -4902,7 +4917,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>322</v>
       </c>
@@ -4913,7 +4928,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>144</v>
       </c>
@@ -4924,7 +4939,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>482</v>
       </c>
@@ -4935,7 +4950,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="184" spans="1:3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>481</v>
       </c>
@@ -4946,7 +4961,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="185" spans="1:3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>278</v>
       </c>
@@ -4957,7 +4972,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>291</v>
       </c>
@@ -4968,7 +4983,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="187" spans="1:3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>538</v>
       </c>
@@ -4979,7 +4994,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>513</v>
       </c>
@@ -4990,7 +5005,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>514</v>
       </c>
@@ -5001,7 +5016,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="190" spans="1:3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>515</v>
       </c>
@@ -5012,7 +5027,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="191" spans="1:3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>9</v>
       </c>
@@ -5023,7 +5038,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="192" spans="1:3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>9</v>
       </c>
@@ -5034,7 +5049,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="193" spans="1:3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>459</v>
       </c>
@@ -5045,7 +5060,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="194" spans="1:3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>459</v>
       </c>
@@ -5056,7 +5071,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="195" spans="1:3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>528</v>
       </c>
@@ -5067,7 +5082,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="196" spans="1:3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>458</v>
       </c>
@@ -5078,7 +5093,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="197" spans="1:3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>493</v>
       </c>
@@ -5089,7 +5104,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="198" spans="1:3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>212</v>
       </c>
@@ -5100,7 +5115,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>35</v>
       </c>
@@ -5111,7 +5126,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="200" spans="1:3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>101</v>
       </c>
@@ -5122,7 +5137,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="201" spans="1:3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>335</v>
       </c>
@@ -5133,7 +5148,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="202" spans="1:3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>36</v>
       </c>
@@ -5144,7 +5159,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="203" spans="1:3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>56</v>
       </c>
@@ -5155,7 +5170,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="204" spans="1:3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>138</v>
       </c>
@@ -5166,7 +5181,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="205" spans="1:3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>497</v>
       </c>
@@ -5177,7 +5192,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="206" spans="1:3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>195</v>
       </c>
@@ -5188,7 +5203,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="207" spans="1:3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>141</v>
       </c>
@@ -5199,7 +5214,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="208" spans="1:3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>143</v>
       </c>
@@ -5210,7 +5225,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="209" spans="1:3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>18</v>
       </c>
@@ -5221,7 +5236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="210" spans="1:3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>154</v>
       </c>
@@ -5232,7 +5247,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="211" spans="1:3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>342</v>
       </c>
@@ -5243,7 +5258,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="212" spans="1:3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>75</v>
       </c>
@@ -5254,7 +5269,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="213" spans="1:3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>129</v>
       </c>
@@ -5265,7 +5280,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="214" spans="1:3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>199</v>
       </c>
@@ -5276,7 +5291,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="215" spans="1:3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>479</v>
       </c>
@@ -5287,7 +5302,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="216" spans="1:3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>267</v>
       </c>
@@ -5298,7 +5313,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="217" spans="1:3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>556</v>
       </c>
@@ -5309,7 +5324,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="218" spans="1:3">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>409</v>
       </c>
@@ -5320,7 +5335,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="219" spans="1:3">
+    <row r="219" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>269</v>
       </c>
@@ -5331,7 +5346,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="220" spans="1:3">
+    <row r="220" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>233</v>
       </c>
@@ -5342,7 +5357,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="221" spans="1:3">
+    <row r="221" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>501</v>
       </c>
@@ -5353,7 +5368,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="222" spans="1:3">
+    <row r="222" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>502</v>
       </c>
@@ -5364,7 +5379,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="223" spans="1:3">
+    <row r="223" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>503</v>
       </c>
@@ -5375,7 +5390,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="224" spans="1:3">
+    <row r="224" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>504</v>
       </c>
@@ -5386,7 +5401,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="225" spans="1:3">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>505</v>
       </c>
@@ -5397,7 +5412,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="226" spans="1:3">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>506</v>
       </c>
@@ -5408,7 +5423,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="227" spans="1:3">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>78</v>
       </c>
@@ -5419,7 +5434,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="228" spans="1:3">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>14</v>
       </c>
@@ -5430,7 +5445,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="229" spans="1:3">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>339</v>
       </c>
@@ -5441,7 +5456,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="230" spans="1:3">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>406</v>
       </c>
@@ -5452,7 +5467,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="231" spans="1:3">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>420</v>
       </c>
@@ -5463,7 +5478,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="232" spans="1:3">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>192</v>
       </c>
@@ -5474,7 +5489,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="233" spans="1:3">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>289</v>
       </c>
@@ -5485,7 +5500,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="234" spans="1:3">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>170</v>
       </c>
@@ -5496,7 +5511,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="235" spans="1:3">
+    <row r="235" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>201</v>
       </c>
@@ -5507,7 +5522,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="236" spans="1:3">
+    <row r="236" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>255</v>
       </c>
@@ -5518,7 +5533,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="237" spans="1:3">
+    <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>77</v>
       </c>
@@ -5529,7 +5544,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="238" spans="1:3">
+    <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>445</v>
       </c>
@@ -5540,7 +5555,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="239" spans="1:3">
+    <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>272</v>
       </c>
@@ -5551,7 +5566,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="240" spans="1:3">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>250</v>
       </c>
@@ -5562,7 +5577,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>536</v>
       </c>
@@ -5573,7 +5588,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>231</v>
       </c>
@@ -5584,7 +5599,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>475</v>
       </c>
@@ -5595,7 +5610,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>190</v>
       </c>
@@ -5606,7 +5621,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="245" spans="1:3">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>730</v>
       </c>
@@ -5617,7 +5632,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="246" spans="1:3">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>734</v>
       </c>
@@ -5628,7 +5643,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="247" spans="1:3">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>132</v>
       </c>
@@ -5639,7 +5654,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="248" spans="1:3">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>340</v>
       </c>
@@ -5650,7 +5665,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="249" spans="1:3">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>438</v>
       </c>
@@ -5661,7 +5676,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="250" spans="1:3">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>440</v>
       </c>
@@ -5672,7 +5687,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="251" spans="1:3">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>375</v>
       </c>
@@ -5683,7 +5698,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="252" spans="1:3">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>365</v>
       </c>
@@ -5694,7 +5709,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="253" spans="1:3">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>442</v>
       </c>
@@ -5705,7 +5720,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="254" spans="1:3">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
         <v>222</v>
       </c>
@@ -5716,7 +5731,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="255" spans="1:3">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
         <v>456</v>
       </c>
@@ -5727,7 +5742,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="256" spans="1:3">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
         <v>46</v>
       </c>
@@ -5738,7 +5753,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="257" spans="1:3">
+    <row r="257" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
         <v>395</v>
       </c>
@@ -5749,7 +5764,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="258" spans="1:3">
+    <row r="258" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>568</v>
       </c>
@@ -5760,7 +5775,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="259" spans="1:3">
+    <row r="259" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
         <v>266</v>
       </c>
@@ -5771,7 +5786,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="260" spans="1:3">
+    <row r="260" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>16</v>
       </c>
@@ -5782,7 +5797,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="261" spans="1:3">
+    <row r="261" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
         <v>215</v>
       </c>
@@ -5793,7 +5808,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="262" spans="1:3">
+    <row r="262" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
         <v>107</v>
       </c>
@@ -5804,7 +5819,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="263" spans="1:3">
+    <row r="263" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>320</v>
       </c>
@@ -5815,7 +5830,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="264" spans="1:3">
+    <row r="264" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>451</v>
       </c>
@@ -5826,7 +5841,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="265" spans="1:3">
+    <row r="265" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
         <v>579</v>
       </c>
@@ -5837,7 +5852,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="266" spans="1:3">
+    <row r="266" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
         <v>583</v>
       </c>
@@ -5848,7 +5863,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="267" spans="1:3">
+    <row r="267" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
         <v>584</v>
       </c>
@@ -5859,7 +5874,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="268" spans="1:3">
+    <row r="268" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
         <v>586</v>
       </c>
@@ -5870,7 +5885,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="269" spans="1:3">
+    <row r="269" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
         <v>588</v>
       </c>
@@ -5881,7 +5896,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="270" spans="1:3">
+    <row r="270" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A270" s="2" t="s">
         <v>679</v>
       </c>
@@ -5892,7 +5907,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="271" spans="1:3">
+    <row r="271" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
         <v>590</v>
       </c>
@@ -5903,7 +5918,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="272" spans="1:3">
+    <row r="272" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
         <v>594</v>
       </c>
@@ -5914,7 +5929,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="273" spans="1:3">
+    <row r="273" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
         <v>596</v>
       </c>
@@ -5925,7 +5940,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="274" spans="1:3">
+    <row r="274" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
         <v>599</v>
       </c>
@@ -5936,7 +5951,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="275" spans="1:3">
+    <row r="275" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
         <v>603</v>
       </c>
@@ -5947,7 +5962,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="276" spans="1:3">
+    <row r="276" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
         <v>604</v>
       </c>
@@ -5958,7 +5973,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="277" spans="1:3">
+    <row r="277" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
         <v>606</v>
       </c>
@@ -5969,7 +5984,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="278" spans="1:3">
+    <row r="278" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A278" s="2" t="s">
         <v>608</v>
       </c>
@@ -5980,7 +5995,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="279" spans="1:3">
+    <row r="279" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A279" s="2" t="s">
         <v>610</v>
       </c>
@@ -5991,7 +6006,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="280" spans="1:3">
+    <row r="280" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A280" s="2" t="s">
         <v>612</v>
       </c>
@@ -6002,7 +6017,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="281" spans="1:3">
+    <row r="281" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A281" s="2" t="s">
         <v>614</v>
       </c>
@@ -6013,7 +6028,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="282" spans="1:3">
+    <row r="282" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A282" s="2" t="s">
         <v>616</v>
       </c>
@@ -6024,7 +6039,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="283" spans="1:3">
+    <row r="283" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A283" s="2" t="s">
         <v>618</v>
       </c>
@@ -6035,7 +6050,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="284" spans="1:3">
+    <row r="284" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A284" s="2" t="s">
         <v>621</v>
       </c>
@@ -6046,7 +6061,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="285" spans="1:3">
+    <row r="285" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A285" s="2" t="s">
         <v>623</v>
       </c>
@@ -6057,7 +6072,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="286" spans="1:3">
+    <row r="286" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A286" s="2" t="s">
         <v>624</v>
       </c>
@@ -6068,7 +6083,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="287" spans="1:3">
+    <row r="287" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A287" s="2" t="s">
         <v>627</v>
       </c>
@@ -6079,7 +6094,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="288" spans="1:3">
+    <row r="288" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A288" s="2" t="s">
         <v>629</v>
       </c>
@@ -6090,7 +6105,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="289" spans="1:3">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A289" s="2" t="s">
         <v>631</v>
       </c>
@@ -6101,7 +6116,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="290" spans="1:3">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
         <v>632</v>
       </c>
@@ -6112,7 +6127,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="291" spans="1:3">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A291" s="2" t="s">
         <v>633</v>
       </c>
@@ -6123,7 +6138,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="292" spans="1:3" ht="93.6">
+    <row r="292" spans="1:3" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A292" s="2" t="s">
         <v>635</v>
       </c>
@@ -6134,7 +6149,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="293" spans="1:3" ht="144" customHeight="1">
+    <row r="293" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A293" s="2" t="s">
         <v>642</v>
       </c>
@@ -6145,7 +6160,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="294" spans="1:3" ht="17.399999999999999" customHeight="1">
+    <row r="294" spans="1:3" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A294" s="2" t="s">
         <v>643</v>
       </c>
@@ -6156,7 +6171,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="295" spans="1:3">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A295" s="2" t="s">
         <v>645</v>
       </c>
@@ -6167,7 +6182,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="296" spans="1:3">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A296" s="2" t="s">
         <v>647</v>
       </c>
@@ -6178,7 +6193,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="297" spans="1:3">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A297" s="2" t="s">
         <v>649</v>
       </c>
@@ -6189,7 +6204,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="298" spans="1:3">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
         <v>654</v>
       </c>
@@ -6200,7 +6215,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="299" spans="1:3">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A299" s="2" t="s">
         <v>656</v>
       </c>
@@ -6211,7 +6226,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="300" spans="1:3">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A300" s="2" t="s">
         <v>657</v>
       </c>
@@ -6222,7 +6237,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="301" spans="1:3">
+    <row r="301" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A301" s="2" t="s">
         <v>659</v>
       </c>
@@ -6233,7 +6248,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="302" spans="1:3" ht="140.4">
+    <row r="302" spans="1:3" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A302" s="2" t="s">
         <v>661</v>
       </c>
@@ -6244,7 +6259,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="303" spans="1:3" ht="196.2" customHeight="1">
+    <row r="303" spans="1:3" ht="196.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A303" s="2" t="s">
         <v>664</v>
       </c>
@@ -6255,7 +6270,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="304" spans="1:3">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A304" s="2" t="s">
         <v>665</v>
       </c>
@@ -6266,7 +6281,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="305" spans="1:3">
+    <row r="305" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A305" s="2" t="s">
         <v>667</v>
       </c>
@@ -6277,7 +6292,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="306" spans="1:3">
+    <row r="306" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A306" s="2" t="s">
         <v>669</v>
       </c>
@@ -6288,7 +6303,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="307" spans="1:3">
+    <row r="307" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A307" s="2" t="s">
         <v>673</v>
       </c>
@@ -6299,7 +6314,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="308" spans="1:3">
+    <row r="308" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A308" s="2" t="s">
         <v>678</v>
       </c>
@@ -6310,7 +6325,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="309" spans="1:3">
+    <row r="309" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A309" s="2" t="s">
         <v>682</v>
       </c>
@@ -6321,7 +6336,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="310" spans="1:3">
+    <row r="310" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A310" s="2" t="s">
         <v>685</v>
       </c>
@@ -6332,7 +6347,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="311" spans="1:3">
+    <row r="311" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A311" s="2" t="s">
         <v>686</v>
       </c>
@@ -6343,7 +6358,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="312" spans="1:3">
+    <row r="312" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A312" s="2" t="s">
         <v>495</v>
       </c>
@@ -6354,7 +6369,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="313" spans="1:3">
+    <row r="313" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A313" s="2" t="s">
         <v>688</v>
       </c>
@@ -6365,7 +6380,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="314" spans="1:3">
+    <row r="314" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A314" s="2" t="s">
         <v>690</v>
       </c>
@@ -6376,7 +6391,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="315" spans="1:3">
+    <row r="315" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A315" s="2" t="s">
         <v>693</v>
       </c>
@@ -6387,7 +6402,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="316" spans="1:3">
+    <row r="316" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A316" s="2" t="s">
         <v>694</v>
       </c>
@@ -6398,7 +6413,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="317" spans="1:3">
+    <row r="317" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A317" s="2" t="s">
         <v>698</v>
       </c>
@@ -6409,7 +6424,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="318" spans="1:3">
+    <row r="318" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A318" s="2" t="s">
         <v>699</v>
       </c>
@@ -6420,7 +6435,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="319" spans="1:3">
+    <row r="319" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A319" s="2" t="s">
         <v>702</v>
       </c>
@@ -6431,7 +6446,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="320" spans="1:3">
+    <row r="320" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A320" s="2" t="s">
         <v>704</v>
       </c>
@@ -6442,7 +6457,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="321" spans="1:3" ht="62.4">
+    <row r="321" spans="1:3" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A321" s="2" t="s">
         <v>710</v>
       </c>
@@ -6453,7 +6468,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="322" spans="1:3">
+    <row r="322" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A322" s="2" t="s">
         <v>711</v>
       </c>
@@ -6464,7 +6479,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="323" spans="1:3">
+    <row r="323" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A323" s="2" t="s">
         <v>713</v>
       </c>
@@ -6475,7 +6490,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="324" spans="1:3">
+    <row r="324" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A324" s="2" t="s">
         <v>716</v>
       </c>
@@ -6486,7 +6501,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="325" spans="1:3">
+    <row r="325" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A325" s="23" t="s">
         <v>718</v>
       </c>
@@ -6497,7 +6512,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="326" spans="1:3">
+    <row r="326" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A326" s="2" t="s">
         <v>719</v>
       </c>
@@ -6508,7 +6523,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="327" spans="1:3">
+    <row r="327" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A327" s="2" t="s">
         <v>720</v>
       </c>
@@ -6519,7 +6534,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="328" spans="1:3">
+    <row r="328" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A328" s="2" t="s">
         <v>253</v>
       </c>
@@ -6530,7 +6545,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="329" spans="1:3">
+    <row r="329" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A329" s="2" t="s">
         <v>721</v>
       </c>
@@ -6541,7 +6556,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="330" spans="1:3">
+    <row r="330" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A330" s="2" t="s">
         <v>728</v>
       </c>
@@ -6552,7 +6567,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="331" spans="1:3">
+    <row r="331" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A331" s="2" t="s">
         <v>731</v>
       </c>
@@ -6563,7 +6578,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="332" spans="1:3">
+    <row r="332" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A332" s="2" t="s">
         <v>727</v>
       </c>
@@ -6574,7 +6589,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="333" spans="1:3">
+    <row r="333" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A333" s="2" t="s">
         <v>248</v>
       </c>
@@ -6585,7 +6600,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="334" spans="1:3">
+    <row r="334" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A334" s="2" t="s">
         <v>726</v>
       </c>
@@ -6596,7 +6611,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="335" spans="1:3">
+    <row r="335" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A335" s="2" t="s">
         <v>722</v>
       </c>
@@ -6607,7 +6622,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="336" spans="1:3">
+    <row r="336" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A336" s="2" t="s">
         <v>407</v>
       </c>
@@ -6618,7 +6633,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="337" spans="1:3">
+    <row r="337" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A337" s="2" t="s">
         <v>736</v>
       </c>
@@ -6629,7 +6644,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="338" spans="1:3">
+    <row r="338" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A338" s="2" t="s">
         <v>738</v>
       </c>
@@ -6638,6 +6653,17 @@
       </c>
       <c r="C338" s="3" t="s">
         <v>739</v>
+      </c>
+    </row>
+    <row r="339" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A339" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="B339" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="C339" s="3" t="s">
+        <v>743</v>
       </c>
     </row>
   </sheetData>
@@ -6658,7 +6684,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="29.5546875" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" customWidth="1"/>
@@ -6668,7 +6694,7 @@
     <col min="8" max="8" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="25" t="s">
         <v>399</v>
       </c>
@@ -6677,28 +6703,28 @@
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
     </row>
-    <row r="7" spans="1:11" ht="27.6" customHeight="1">
+    <row r="7" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
         <v>397</v>
       </c>
@@ -6709,7 +6735,7 @@
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
     </row>
-    <row r="8" spans="1:11" s="11" customFormat="1" ht="64.2" customHeight="1">
+    <row r="8" spans="1:11" s="11" customFormat="1" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
         <v>390</v>
@@ -6730,7 +6756,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="7" customFormat="1" ht="38.4" customHeight="1">
+    <row r="9" spans="1:11" s="7" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>392</v>
       </c>
@@ -6758,7 +6784,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" s="7" customFormat="1" ht="38.4" customHeight="1">
+    <row r="10" spans="1:11" s="7" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>394</v>
       </c>
@@ -6786,7 +6812,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" s="7" customFormat="1" ht="28.2" customHeight="1">
+    <row r="11" spans="1:11" s="7" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -6801,7 +6827,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="12" spans="1:11" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -6815,7 +6841,7 @@
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:11" s="14" customFormat="1" ht="23.4" customHeight="1">
+    <row r="13" spans="1:11" s="14" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F13" s="17">
         <f>F12*F11</f>
         <v>118826</v>
@@ -6826,7 +6852,7 @@
         <v>227002.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="14" customFormat="1" ht="17.399999999999999"/>
+    <row r="14" spans="1:11" s="14" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C7:F7"/>
@@ -6845,7 +6871,7 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="29.5546875" customWidth="1"/>
     <col min="4" max="4" width="12.5546875" customWidth="1"/>
@@ -6855,35 +6881,35 @@
     <col min="8" max="8" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
       <c r="F3" s="25"/>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="25"/>
       <c r="C4" s="25"/>
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
     </row>
-    <row r="7" spans="1:11" ht="27.6" customHeight="1">
+    <row r="7" spans="1:11" ht="27.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
         <v>397</v>
       </c>
@@ -6894,7 +6920,7 @@
       <c r="E7" s="24"/>
       <c r="F7" s="24"/>
     </row>
-    <row r="8" spans="1:11" s="11" customFormat="1" ht="64.2" customHeight="1">
+    <row r="8" spans="1:11" s="11" customFormat="1" ht="64.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
         <v>390</v>
@@ -6915,7 +6941,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="7" customFormat="1" ht="45" customHeight="1">
+    <row r="9" spans="1:11" s="7" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>392</v>
       </c>
@@ -6943,7 +6969,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" s="7" customFormat="1" ht="38.4" customHeight="1">
+    <row r="10" spans="1:11" s="7" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>394</v>
       </c>
@@ -6971,7 +6997,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" s="7" customFormat="1" ht="28.2" customHeight="1">
+    <row r="11" spans="1:11" s="7" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
@@ -6986,7 +7012,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="14" customFormat="1" ht="39" customHeight="1">
+    <row r="12" spans="1:11" s="14" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -7000,7 +7026,7 @@
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
     </row>
-    <row r="13" spans="1:11" s="14" customFormat="1" ht="23.4" customHeight="1">
+    <row r="13" spans="1:11" s="14" customFormat="1" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F13" s="17">
         <f>F12*F11</f>
         <v>145730</v>
@@ -7011,8 +7037,8 @@
         <v>307714.5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="18" customFormat="1" ht="17.399999999999999"/>
-    <row r="15" spans="1:11" s="19" customFormat="1" ht="18">
+    <row r="14" spans="1:11" s="18" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:11" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="E15" s="20">
         <v>130</v>
       </c>
@@ -7021,7 +7047,7 @@
         <v>72865</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="19" customFormat="1" ht="18">
+    <row r="16" spans="1:11" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="E16" s="20">
         <v>212</v>
       </c>
@@ -7030,7 +7056,7 @@
         <v>118826</v>
       </c>
     </row>
-    <row r="17" spans="5:6" s="19" customFormat="1" ht="18">
+    <row r="17" spans="5:6" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="E17" s="20">
         <f>E16-E15</f>
         <v>82</v>

</xml_diff>